<commit_message>
Space out the MOSFETs better
They were pretty close. Space them out better so that the power rail
routing can be cleaner.

Signed-off-by: Grant Likely <grant.likely@linaro.org>
</commit_message>
<xml_diff>
--- a/Sensors-bom-test.xlsx
+++ b/Sensors-bom-test.xlsx
@@ -172,7 +172,7 @@
     <t>Yxcon</t>
   </si>
   <si>
-    <t>F243-1220xxxSUx1</t>
+    <t>F243-1220xxxSUx1 – 8mm pin length</t>
   </si>
   <si>
     <t>J1 P10</t>
@@ -948,15 +948,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>228240</xdr:colOff>
+      <xdr:colOff>255240</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>43560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4048200</xdr:colOff>
+      <xdr:colOff>4074840</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -969,8 +969,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="228240" y="16449480"/>
-          <a:ext cx="5083920" cy="5248800"/>
+          <a:off x="255240" y="16440480"/>
+          <a:ext cx="5083560" cy="5248440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -993,7 +993,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Update testplan and manufacturing files for revB
Ready for manufacturing (finally!)

Signed-off-by: Grant Likely <grant.likely@linaro.org>
</commit_message>
<xml_diff>
--- a/Sensors-bom-test.xlsx
+++ b/Sensors-bom-test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="252">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -172,7 +172,7 @@
     <t>Yxcon</t>
   </si>
   <si>
-    <t>F243-1220xxxSUx1 – 8mm pin length</t>
+    <t>F243-1220xxxSUx1 8mm pins</t>
   </si>
   <si>
     <t>J1 P10</t>
@@ -286,7 +286,25 @@
     <t>RC0603JR-07220RL</t>
   </si>
   <si>
-    <t>R2 R3 R5 R7 R13 R14</t>
+    <t>R2 R3 R4 R13 R14</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>RC0402JR-071KL</t>
+  </si>
+  <si>
+    <t>R19 R20</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>RC0603FR-07100KL</t>
+  </si>
+  <si>
+    <t>R5 R7</t>
   </si>
   <si>
     <t>620R</t>
@@ -295,34 +313,7 @@
     <t>RC0603JR-07620RL</t>
   </si>
   <si>
-    <t>R15 R16 R17 R18 R21 R22 R23 R24</t>
-  </si>
-  <si>
-    <t>2.2K</t>
-  </si>
-  <si>
-    <t>RC0603JR-072K2L</t>
-  </si>
-  <si>
-    <t>R19 R20</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>RC0603FR-07100KL</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>RC0402JR-071KL</t>
-  </si>
-  <si>
-    <t>R8 R10</t>
+    <t>R8 R10 R15 R16 R17 R18</t>
   </si>
   <si>
     <t>22R</t>
@@ -655,7 +646,7 @@
     <t>Pin 40</t>
   </si>
   <si>
-    <t>Short together the two pads on J1. (perhaps using a jig with pogopins? Could use some advice on the best way to do this. J1 is only used for manufacturing testing)</t>
+    <t>Short together the two pads on J1.</t>
   </si>
   <si>
     <t>DPDT position labels</t>
@@ -733,7 +724,7 @@
     <t>j.</t>
   </si>
   <si>
-    <t>Connect GROVE LED modules to connectors P8-11, P14-16 and P18. 8 modules in all (or use a single module to test each connector one at a time.)</t>
+    <t>Connect GROVE LED modules to connectors D3-D7, A0-A2, A6 and I2C-AT. 10 modules in all (or use a single module to test each connector one at a time.)</t>
   </si>
   <si>
     <t>Note:</t>
@@ -751,19 +742,19 @@
     <t>l.</t>
   </si>
   <si>
-    <t>Connect GROVE cable from P14 to P12</t>
+    <t>Connect GROVE cable from D3 to GPIO1</t>
   </si>
   <si>
     <t>m.</t>
   </si>
   <si>
-    <t>Connect GROVE cable from P15 to P19</t>
+    <t>Connect GROVE cable from D5 to GPIO2</t>
   </si>
   <si>
     <t>n.</t>
   </si>
   <si>
-    <t>Verify UUT LEDs are flashing: D4-D7 (GPIOA-GPIOD)</t>
+    <t>Verify UUT LEDs are flashing: D1 &amp; D2 (GPIOs A &amp; B)</t>
   </si>
   <si>
     <t>o.</t>
@@ -866,13 +857,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -895,8 +890,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -927,8 +922,8 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -948,15 +943,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>255240</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:colOff>282240</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4074840</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>148680</xdr:rowOff>
+      <xdr:colOff>4101480</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>126720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -969,8 +964,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="255240" y="16440480"/>
-          <a:ext cx="5083560" cy="5248440"/>
+          <a:off x="282240" y="16431480"/>
+          <a:ext cx="5083200" cy="5248080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -990,10 +985,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1005,11 +1000,12 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6444444444444"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.7"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.83333333333333"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="12.3"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.83333333333333"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0"/>
@@ -1017,11 +1013,11 @@
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="0"/>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="0"/>
@@ -1030,36 +1026,37 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="0"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" s="9" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -1077,12 +1074,13 @@
       <c r="F5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="2" t="n">
         <v>302010126</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="H5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -1100,12 +1098,13 @@
       <c r="F6" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="G6" s="2" t="n">
         <v>302010138</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="H6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -1123,12 +1122,13 @@
       <c r="F7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="7" t="n">
+      <c r="G7" s="2" t="n">
         <v>302010148</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="H7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -1146,12 +1146,13 @@
       <c r="F8" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="7" t="n">
+      <c r="G8" s="2" t="n">
         <v>302010143</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="H8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -1169,12 +1170,13 @@
       <c r="F9" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="7" t="n">
+      <c r="G9" s="2" t="n">
         <v>320010015</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="H9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -1192,12 +1194,13 @@
       <c r="F10" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="7" t="n">
+      <c r="G10" s="2" t="n">
         <v>304090045</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="H10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -1215,12 +1218,13 @@
       <c r="F11" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="7" t="n">
+      <c r="G11" s="2" t="n">
         <v>304090042</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="H11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="0" t="n">
@@ -1238,12 +1242,13 @@
       <c r="F12" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="7" t="n">
+      <c r="G12" s="2" t="n">
         <v>304090043</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="H12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B13" s="0" t="n">
@@ -1261,12 +1266,13 @@
       <c r="F13" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="7" t="n">
+      <c r="G13" s="2" t="n">
         <v>310010049</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="H13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="0" t="n">
@@ -1284,10 +1290,11 @@
       <c r="F14" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="G14" s="2"/>
+      <c r="H14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="0" t="n">
@@ -1300,10 +1307,11 @@
         <v>54</v>
       </c>
       <c r="F15" s="0"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="G15" s="2"/>
+      <c r="H15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="0" t="n">
@@ -1321,12 +1329,13 @@
       <c r="F16" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="7" t="n">
+      <c r="G16" s="2" t="n">
         <v>320110032</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="H16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B17" s="0" t="n">
@@ -1344,12 +1353,13 @@
       <c r="F17" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="7" t="n">
+      <c r="G17" s="2" t="n">
         <v>320110033</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="H17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B18" s="0" t="n">
@@ -1367,12 +1377,13 @@
       <c r="F18" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G18" s="7" t="n">
+      <c r="G18" s="2" t="n">
         <v>320030003</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="H18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="0" t="n">
@@ -1390,12 +1401,13 @@
       <c r="F19" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="G19" s="7" t="n">
+      <c r="G19" s="2" t="n">
         <v>320030039</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="H19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B20" s="0" t="n">
@@ -1413,12 +1425,13 @@
       <c r="F20" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="G20" s="7" t="n">
+      <c r="G20" s="2" t="n">
         <v>320030004</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="H20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
         <v>75</v>
       </c>
       <c r="B21" s="0" t="n">
@@ -1436,12 +1449,13 @@
       <c r="F21" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="G21" s="7" t="n">
+      <c r="G21" s="2" t="n">
         <v>320020003</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="H21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
         <v>79</v>
       </c>
       <c r="B22" s="0" t="n">
@@ -1459,12 +1473,13 @@
       <c r="F22" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="G22" s="7" t="n">
+      <c r="G22" s="2" t="n">
         <v>305010017</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="H22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="s">
         <v>83</v>
       </c>
       <c r="B23" s="0" t="n">
@@ -1482,12 +1497,13 @@
       <c r="F23" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="G23" s="7" t="n">
+      <c r="G23" s="2" t="n">
         <v>305030014</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="H23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
         <v>85</v>
       </c>
       <c r="B24" s="0" t="n">
@@ -1505,16 +1521,17 @@
       <c r="F24" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="G24" s="7" t="n">
+      <c r="G24" s="2" t="n">
         <v>301010163</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="H24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
         <v>89</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>90</v>
@@ -1528,16 +1545,17 @@
       <c r="F25" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="G25" s="7" t="n">
-        <v>301010210</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="G25" s="2" t="n">
+        <v>301010006</v>
+      </c>
+      <c r="H25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
         <v>92</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>93</v>
@@ -1551,12 +1569,13 @@
       <c r="F26" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="G26" s="7" t="n">
-        <v>301010124</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="G26" s="2" t="n">
+        <v>301010196</v>
+      </c>
+      <c r="H26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
         <v>95</v>
       </c>
       <c r="B27" s="0" t="n">
@@ -1574,16 +1593,17 @@
       <c r="F27" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="G27" s="7" t="n">
-        <v>301010196</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="G27" s="2" t="n">
+        <v>301010210</v>
+      </c>
+      <c r="H27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
         <v>98</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>99</v>
@@ -1592,21 +1612,22 @@
         <v>87</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="G28" s="7" t="n">
-        <v>301010006</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="G28" s="2" t="n">
+        <v>301010289</v>
+      </c>
+      <c r="H28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
         <v>101</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>102</v>
@@ -1620,150 +1641,157 @@
       <c r="F29" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G29" s="7" t="n">
-        <v>301010289</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="G29" s="2" t="n">
+        <v>301010299</v>
+      </c>
+      <c r="H29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
         <v>104</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>105</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="G30" s="7" t="n">
-        <v>301010299</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>311010004</v>
+      </c>
+      <c r="H30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E31" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="F31" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G31" s="7" t="n">
-        <v>311010004</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>112</v>
+      <c r="G31" s="2" t="n">
+        <v>310030097</v>
+      </c>
+      <c r="H31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>115</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="G32" s="7" t="n">
-        <v>310030097</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
         <v>116</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>310030016</v>
+      </c>
+      <c r="H32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="G33" s="7" t="n">
-        <v>310030016</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>310070030</v>
+      </c>
+      <c r="H33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E34" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="F34" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="G34" s="7" t="n">
-        <v>310070030</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>125</v>
+      <c r="G34" s="2" t="n">
+        <v>310050024</v>
+      </c>
+      <c r="H34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E35" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F35" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="F35" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="G35" s="7" t="n">
-        <v>310050024</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="G35" s="2" t="n">
+        <v>310050026</v>
+      </c>
+      <c r="H35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8" t="s">
         <v>129</v>
       </c>
       <c r="B36" s="0" t="n">
@@ -1773,73 +1801,58 @@
         <v>130</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="G36" s="7" t="n">
-        <v>310050026</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="G36" s="2" t="n">
+        <v>306010054</v>
+      </c>
+      <c r="H36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="B37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="G37" s="7" t="n">
-        <v>306010054</v>
-      </c>
+      <c r="A37" s="0"/>
+      <c r="B37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="G37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="4"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="4"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E41" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>138</v>
+        <v>134</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F42" s="9" t="s">
-        <v>139</v>
+      <c r="F42" s="10" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1872,14 +1885,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>140</v>
+      <c r="A1" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="B1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>141</v>
+      <c r="A2" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="B2" s="0"/>
     </row>
@@ -1888,89 +1901,89 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>143</v>
+        <v>139</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B6" s="9" t="n">
+        <v>143</v>
+      </c>
+      <c r="B6" s="10" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>156</v>
+        <v>152</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B14" s="9"/>
+        <v>157</v>
+      </c>
+      <c r="B14" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1990,26 +2003,26 @@
   </sheetPr>
   <dimension ref="A1:B65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="A66"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="13.0074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="52.1444444444444"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="13.0074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="52.1444444444444"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.83333333333333"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>161</v>
+      <c r="A1" s="13" t="s">
+        <v>158</v>
       </c>
       <c r="B1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>141</v>
+      <c r="A2" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="B2" s="0"/>
     </row>
@@ -2018,8 +2031,8 @@
       <c r="B3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>162</v>
+      <c r="A4" s="13" t="s">
+        <v>159</v>
       </c>
       <c r="B4" s="0"/>
     </row>
@@ -2028,445 +2041,445 @@
       <c r="B5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15"/>
+      <c r="B8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="B6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
+      <c r="B10" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="B7" s="13"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14"/>
-      <c r="B8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13"/>
+      <c r="B11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
+      <c r="B12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12"/>
-      <c r="B11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
+      <c r="B14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
+      <c r="B15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
+      <c r="B16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15"/>
+      <c r="B17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="B14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
+      <c r="B18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="B15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
+      <c r="B19" s="14"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14"/>
-      <c r="B17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="s">
+      <c r="B20" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="B18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B19" s="13"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
+      <c r="B21" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B22" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
+    <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
+      <c r="B23" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="B22" s="15" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="15" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="s">
+      <c r="B24" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="B23" s="15" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="15" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14" t="s">
+      <c r="B25" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B24" s="15" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="15" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14" t="s">
+      <c r="B26" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="B25" s="15" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="15" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14" t="s">
+      <c r="B27" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="B26" s="15" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="15" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="14" t="s">
+      <c r="B28" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="B27" s="15" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="15" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14" t="s">
+      <c r="B29" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="B28" s="15" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="15" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14" t="s">
+      <c r="B30" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="B29" s="15" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="15" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="14" t="s">
+      <c r="B31" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="B30" s="15" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="15" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="14" t="s">
+      <c r="B32" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="B31" s="15" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="15" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14" t="s">
+      <c r="B33" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="B32" s="15" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="15" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
+      <c r="B34" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="B33" s="15" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="15" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
+      <c r="B35" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B34" s="15" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="15" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14" t="s">
+      <c r="B36" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="B35" s="15" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="15" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="14" t="s">
+      <c r="B37" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B36" s="15" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="15" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="14" t="s">
+      <c r="B38" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B39" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="15"/>
+      <c r="B40" s="8"/>
+    </row>
+    <row r="41" s="11" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="16" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="14" t="s">
+      <c r="B41" s="16"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="15"/>
+      <c r="B42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="B38" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="14" t="s">
+      <c r="B43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="B39" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="14"/>
-      <c r="B40" s="15"/>
-    </row>
-    <row r="41" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="13" t="s">
+      <c r="B44" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="B41" s="13"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14"/>
-      <c r="B42" s="0"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="14" t="s">
+    </row>
+    <row r="45" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="B43" s="0"/>
-    </row>
-    <row r="44" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14" t="s">
+      <c r="B45" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="B44" s="15" t="s">
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="15"/>
+      <c r="B46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="13" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="14" t="s">
+      <c r="B47" s="0"/>
+    </row>
+    <row r="48" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B48" s="8" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="14"/>
-      <c r="B46" s="0"/>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="12" t="s">
+    <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="B47" s="0"/>
-    </row>
-    <row r="48" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="14" t="s">
+      <c r="B49" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="B48" s="15" t="s">
+    </row>
+    <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="15" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="14" t="s">
+      <c r="B50" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="B49" s="15" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="15" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="14" t="s">
+      <c r="B51" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="B50" s="15" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="15" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="14" t="s">
+      <c r="B52" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="B51" s="15" t="s">
+    </row>
+    <row r="53" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="15" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="14" t="s">
+      <c r="B53" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="B52" s="15" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="15" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="14" t="s">
+      <c r="B54" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="B53" s="15" t="s">
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="15" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="14" t="s">
+      <c r="B55" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="B54" s="15" t="s">
+    </row>
+    <row r="56" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="15" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="14" t="s">
+      <c r="B56" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="B55" s="0" t="s">
+    </row>
+    <row r="57" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="15" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="14" t="s">
+      <c r="B57" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="B56" s="15" t="s">
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="15"/>
+      <c r="B58" s="0"/>
+    </row>
+    <row r="59" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="13" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="14" t="s">
+      <c r="B59" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="B57" s="15" t="s">
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="15" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="14"/>
-      <c r="B58" s="0"/>
-    </row>
-    <row r="59" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="12" t="s">
+      <c r="B60" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="B59" s="15" t="s">
+    </row>
+    <row r="61" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="15" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="14" t="s">
+      <c r="B61" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="B60" s="0" t="s">
+    </row>
+    <row r="62" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="15" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="14" t="s">
+      <c r="B62" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="B61" s="15" t="s">
+    </row>
+    <row r="63" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="15" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="14" t="s">
+      <c r="B63" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="B62" s="15" t="s">
+    </row>
+    <row r="64" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="15" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="14" t="s">
+      <c r="B64" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="B63" s="15" t="s">
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="15" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="14" t="s">
+      <c r="B65" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="B64" s="15" t="s">
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="15"/>
+      <c r="B66" s="8"/>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="15"/>
+      <c r="B67" s="0"/>
+    </row>
+    <row r="68" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="15" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="14" t="s">
+      <c r="B68" s="8" t="s">
         <v>251</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="14"/>
-      <c r="B66" s="15"/>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="14"/>
-      <c r="B67" s="0"/>
-    </row>
-    <row r="68" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update rev C design files
Signed-off-by: Grant Likely <grant.likely@linaro.org>
</commit_message>
<xml_diff>
--- a/Sensors-bom-test.xlsx
+++ b/Sensors-bom-test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,15 +17,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="261">
   <si>
     <t>Bill of Materials</t>
   </si>
   <si>
-    <t>96Boards Sensors Rev B</t>
-  </si>
-  <si>
-    <t>Oct 14 2015</t>
+    <t>96Boards Sensors Rev C</t>
+  </si>
+  <si>
+    <t>Nov 29 2015</t>
   </si>
   <si>
     <t>Reference</t>
@@ -64,7 +64,7 @@
     <t>CC0603JRNPO9BN390</t>
   </si>
   <si>
-    <t>C3 C5 C6 C7 C12 C13 C14 C15 C16 C17 C18</t>
+    <t>C3 C5 C6 C7 C12 C13 C14 C15 C16 C17</t>
   </si>
   <si>
     <t>100n</t>
@@ -73,39 +73,45 @@
     <t>CC0603KRX7R9BB104</t>
   </si>
   <si>
+    <t>C18 C19 C22</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>Capacitors_SMD:C_0805</t>
+  </si>
+  <si>
+    <t>CC0805KKX5R8BB106</t>
+  </si>
+  <si>
     <t>C1 C2 C4</t>
   </si>
   <si>
     <t>2u2</t>
   </si>
   <si>
-    <t>Capacitors_SMD:C_0805</t>
-  </si>
-  <si>
     <t>CC0805KKX7R8BB225</t>
   </si>
   <si>
+    <t>C20 C21</t>
+  </si>
+  <si>
+    <t>100p</t>
+  </si>
+  <si>
+    <t>CC0603JRNPO9BN101</t>
+  </si>
+  <si>
     <t>C8 C9</t>
   </si>
   <si>
     <t>22p</t>
   </si>
   <si>
-    <t>YAGEO</t>
-  </si>
-  <si>
     <t>CC0603JRNPO9BN220</t>
   </si>
   <si>
-    <t>C19</t>
-  </si>
-  <si>
-    <t>10u</t>
-  </si>
-  <si>
-    <t>CC0805KKX5R8BB106</t>
-  </si>
-  <si>
     <t>CON1</t>
   </si>
   <si>
@@ -154,6 +160,30 @@
     <t>19-217-G7C-AN1P2-3T</t>
   </si>
   <si>
+    <t>G1 D3 I2C0 P9</t>
+  </si>
+  <si>
+    <t>GROVE</t>
+  </si>
+  <si>
+    <t>Sensors:Grove_SMD_Connector</t>
+  </si>
+  <si>
+    <t>Taifeng</t>
+  </si>
+  <si>
+    <t>1125R-SMT-4P</t>
+  </si>
+  <si>
+    <t>A0 A1 G2 A2 G3 G4 D4 D5 D6 D7 I2C1 P8 P13 P14</t>
+  </si>
+  <si>
+    <t>Sensors:Grove4P</t>
+  </si>
+  <si>
+    <t>1125S-4P</t>
+  </si>
+  <si>
     <t>IC1</t>
   </si>
   <si>
@@ -181,40 +211,7 @@
     <t>Yxcon</t>
   </si>
   <si>
-    <t>F243-1220xxxSUx1 8mm pins</t>
-  </si>
-  <si>
-    <t>J1 P10</t>
-  </si>
-  <si>
-    <t>CBUS</t>
-  </si>
-  <si>
-    <t>Sensors:Pin_Header_Straight_1x02_Pitch2mm</t>
-  </si>
-  <si>
-    <t>GPIO1 D3 P9 P11</t>
-  </si>
-  <si>
-    <t>I2C0</t>
-  </si>
-  <si>
-    <t>Sensors:Grove_SMD_Connector</t>
-  </si>
-  <si>
-    <t>Taifeng</t>
-  </si>
-  <si>
-    <t>1125R-SMT-4P</t>
-  </si>
-  <si>
-    <t>A0 A1 GPIO2 A2 GPIO3 D4 D5 D6 A6 D7 P8 P12 P13 P14</t>
-  </si>
-  <si>
-    <t>Sensors:Grove4P</t>
-  </si>
-  <si>
-    <t>1125S-4P</t>
+    <t>F243-1220xxxSUx1 w/ 8mm Pins</t>
   </si>
   <si>
     <t>P2 P5</t>
@@ -256,9 +253,6 @@
     <t>P6 P7</t>
   </si>
   <si>
-    <t>96B_SPI</t>
-  </si>
-  <si>
     <t>Pin_Headers:Pin_Header_Straight_2x03</t>
   </si>
   <si>
@@ -277,12 +271,6 @@
     <t>JCET</t>
   </si>
   <si>
-    <t>Q2 Q3</t>
-  </si>
-  <si>
-    <t>CJ2305</t>
-  </si>
-  <si>
     <t>R11 R12</t>
   </si>
   <si>
@@ -304,13 +292,13 @@
     <t>RC0402JR-071KL</t>
   </si>
   <si>
-    <t>R19 R20</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>RC0603FR-07100KL</t>
+    <t>R15 R22</t>
+  </si>
+  <si>
+    <t>200K</t>
+  </si>
+  <si>
+    <t>RC0603JR-07200KL</t>
   </si>
   <si>
     <t>R5 R7</t>
@@ -322,7 +310,7 @@
     <t>RC0603JR-07620RL</t>
   </si>
   <si>
-    <t>R8 R10 R15 R16 R17 R18</t>
+    <t>R8 R10</t>
   </si>
   <si>
     <t>22R</t>
@@ -331,7 +319,7 @@
     <t>RC0603JR-0722RL</t>
   </si>
   <si>
-    <t>R1 R6 R9</t>
+    <t>R1 R6 R9 R16 R17 R18 R19 R23 R24 R25 R26</t>
   </si>
   <si>
     <t>10K</t>
@@ -340,21 +328,6 @@
     <t>RC0603FR-0710KL</t>
   </si>
   <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>VIO</t>
-  </si>
-  <si>
-    <t>Sensors:DIP_Toggle_Switch</t>
-  </si>
-  <si>
-    <t>Deyilong</t>
-  </si>
-  <si>
-    <t>MS-22D18 G2</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -415,6 +388,18 @@
     <t>TXS0108EPWR</t>
   </si>
   <si>
+    <t>U6 U7</t>
+  </si>
+  <si>
+    <t>PCA9306</t>
+  </si>
+  <si>
+    <t>Sensors:VSSOP-8_2.4x2.1mm_Pitch0.5mm</t>
+  </si>
+  <si>
+    <t>PCA9306DCU</t>
+  </si>
+  <si>
     <t>X1</t>
   </si>
   <si>
@@ -439,21 +424,42 @@
     <t>M2.5 8mm threaded spacer</t>
   </si>
   <si>
+    <t>Changes from Rev B:</t>
+  </si>
+  <si>
     <t>Note</t>
   </si>
   <si>
     <t>Select components as appropriate for cost reductions</t>
   </si>
   <si>
+    <t>C18 changed from 100n to 10u</t>
+  </si>
+  <si>
     <t>Seeed OPL components have been selected where possible</t>
   </si>
   <si>
+    <t>C20 C21 and C22 added</t>
+  </si>
+  <si>
+    <t>R15 changed to 100k</t>
+  </si>
+  <si>
+    <t>R16 R17 R18 R19 changed to 10k</t>
+  </si>
+  <si>
+    <t>Added R22 R23 R24 R25 R26</t>
+  </si>
+  <si>
+    <t>Removed SW1</t>
+  </si>
+  <si>
+    <t>Removed Q2 Q3</t>
+  </si>
+  <si>
     <t>PCB Spec</t>
   </si>
   <si>
-    <t>96Boards Sensors Rev A</t>
-  </si>
-  <si>
     <t>Material</t>
   </si>
   <si>
@@ -545,6 +551,9 @@
   </si>
   <si>
     <t>Power Supplies for +5V and +1.8V</t>
+  </si>
+  <si>
+    <t>Pogo pins or equivalent to mate with J1</t>
   </si>
   <si>
     <t>Design</t>
@@ -908,12 +917,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -922,10 +935,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -961,15 +970,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>336240</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:colOff>363240</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>185400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4154760</xdr:colOff>
+      <xdr:colOff>4181400</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -982,8 +991,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="336240" y="16413480"/>
-          <a:ext cx="5082480" cy="5247360"/>
+          <a:off x="363240" y="16404480"/>
+          <a:ext cx="5082120" cy="5247000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1003,10 +1012,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1073,7 +1082,7 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" s="9" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="8" customFormat="true" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1092,17 +1101,17 @@
       <c r="F5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="8" t="n">
+      <c r="G5" s="0" t="n">
         <v>302010126</v>
       </c>
       <c r="H5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="31.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>16</v>
@@ -1116,11 +1125,11 @@
       <c r="F6" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="8" t="n">
+      <c r="G6" s="0" t="n">
         <v>302010138</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
@@ -1139,531 +1148,534 @@
       <c r="F7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="8" t="n">
-        <v>302010148</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="0" t="n">
+        <v>302010178</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>302010148</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="8" t="n">
+      <c r="E9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>302010076</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>302010143</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="9" t="n">
-        <v>302010178</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="0" t="s">
+    <row r="11" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="8" t="n">
-        <v>320010015</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="G11" s="0" t="n">
+        <v>320010015</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="8" t="n">
-        <v>304090045</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="0" t="s">
+      <c r="G12" s="0" t="n">
+        <v>304090045</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="8" t="n">
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="0" t="n">
         <v>304090042</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="0" t="n">
+    <row r="14" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="8" t="n">
+      <c r="C14" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <v>304090043</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="0" t="n">
+    <row r="15" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>320110032</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>320110033</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="8" t="n">
+      <c r="C17" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <v>310010049</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="0" t="n">
+    <row r="18" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="0"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="0" t="s">
+      <c r="C18" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="D18" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="8" t="n">
-        <v>320110032</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
+      <c r="E18" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="0" t="s">
+      <c r="F18" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="0" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="G18" s="8" t="n">
-        <v>320110033</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="E19" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="0" t="s">
+      <c r="G19" s="0" t="n">
+        <v>320030003</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="G19" s="8" t="n">
-        <v>320030003</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="E20" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="0" t="s">
+      <c r="G20" s="0" t="n">
+        <v>320030039</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="G20" s="8" t="n">
-        <v>320030039</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="E21" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="0" t="s">
+      <c r="G21" s="0" t="n">
+        <v>320030004</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="G21" s="8" t="n">
-        <v>320030004</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="D22" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="G22" s="0" t="n">
+        <v>320020003</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="8" t="n">
-        <v>320020003</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="F23" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>305010017</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="G23" s="8" t="n">
-        <v>305010017</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="G24" s="8" t="n">
-        <v>305030014</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="0" t="n">
+        <v>301010163</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>89</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F25" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>301010006</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G25" s="8" t="n">
-        <v>301010163</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
+      <c r="B26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="B26" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>93</v>
-      </c>
       <c r="D26" s="0" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>301010212</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="G26" s="8" t="n">
-        <v>301010006</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="0" t="s">
+      <c r="G27" s="0" t="n">
+        <v>301010210</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="G27" s="8" t="n">
-        <v>301010196</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>98</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="0" t="s">
+      <c r="G28" s="0" t="n">
+        <v>301010289</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G28" s="8" t="n">
-        <v>301010210</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
+      <c r="B29" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>102</v>
-      </c>
       <c r="D29" s="0" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F29" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>301010299</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="G29" s="8" t="n">
-        <v>301010289</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C30" s="0" t="s">
+      <c r="D30" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="E30" s="0" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="G30" s="8" t="n">
-        <v>301010299</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>104</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>310030097</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
         <v>107</v>
       </c>
@@ -1674,42 +1686,42 @@
         <v>108</v>
       </c>
       <c r="D31" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="F31" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="G31" s="0" t="n">
+        <v>310030016</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="G31" s="8" t="n">
-        <v>311010004</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C32" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="E32" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="F32" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="F32" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="G32" s="8" t="n">
-        <v>310030097</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="0" t="n">
+        <v>310070030</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
         <v>116</v>
       </c>
@@ -1720,19 +1732,19 @@
         <v>117</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="G33" s="8" t="n">
-        <v>310030016</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>117</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>310050024</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
         <v>120</v>
       </c>
@@ -1743,103 +1755,84 @@
         <v>121</v>
       </c>
       <c r="D34" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="G34" s="0" t="n">
+        <v>310050026</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="B35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="G34" s="8" t="n">
-        <v>310070030</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
+      <c r="D35" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>127</v>
-      </c>
       <c r="E35" s="0" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="G35" s="8" t="n">
-        <v>310050024</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="36" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C36" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>130</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>128</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="G36" s="8" t="n">
-        <v>310050026</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="G37" s="8" t="n">
+      <c r="G36" s="0" t="n">
         <v>306010054</v>
       </c>
     </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7"/>
+      <c r="B37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="G37" s="9"/>
+    </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="0"/>
       <c r="D38" s="0"/>
       <c r="F38" s="0"/>
-      <c r="G38" s="8"/>
+      <c r="G38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4"/>
@@ -1848,13 +1841,13 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4"/>
@@ -1865,16 +1858,52 @@
       <c r="F41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="E42" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="F42" s="10" t="s">
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F43" s="10" t="s">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1895,8 +1924,8 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1908,13 +1937,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>144</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0"/>
     </row>
@@ -1923,89 +1952,89 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B6" s="10" t="n">
+        <v>151</v>
+      </c>
+      <c r="B6" s="11" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>153</v>
+        <v>154</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>161</v>
+        <v>164</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="B14" s="10"/>
+        <v>165</v>
+      </c>
+      <c r="B14" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2023,28 +2052,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B65536"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="13.0074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="52.1444444444444"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="13.0074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="52.1444444444444"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.83333333333333"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>144</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0"/>
     </row>
@@ -2054,7 +2083,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="0"/>
     </row>
@@ -2064,13 +2093,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B7" s="14"/>
     </row>
@@ -2080,16 +2109,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2098,69 +2127,67 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15"/>
+      <c r="A17" s="15" t="s">
+        <v>178</v>
+      </c>
       <c r="B17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
-        <v>176</v>
-      </c>
+      <c r="A18" s="15"/>
       <c r="B18" s="0"/>
     </row>
-    <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="B19" s="14"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="B20" s="7" t="s">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="s">
         <v>179</v>
       </c>
+      <c r="B19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>182</v>
@@ -2168,348 +2195,355 @@
     </row>
     <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="15" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="15" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="15" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="15" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="15" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="15" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="15" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="15" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="15" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="15" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="15" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="15" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>179</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="15" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="15"/>
-      <c r="B40" s="7"/>
-    </row>
-    <row r="41" s="11" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="B41" s="16"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="15"/>
-      <c r="B42" s="0"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="15"/>
+      <c r="B41" s="7"/>
+    </row>
+    <row r="42" s="12" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B42" s="16"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="15" t="s">
-        <v>216</v>
-      </c>
+      <c r="A43" s="15"/>
       <c r="B43" s="0"/>
     </row>
-    <row r="44" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>218</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="B44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="15" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="15"/>
-      <c r="B46" s="0"/>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="13" t="s">
-        <v>221</v>
-      </c>
+      <c r="A47" s="15"/>
       <c r="B47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>223</v>
-      </c>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="B48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="15" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="15" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="15" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="15" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="15" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="15" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="B55" s="0" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="B56" s="7" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="15"/>
-      <c r="B58" s="0"/>
-    </row>
-    <row r="59" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="B59" s="7" t="s">
+    </row>
+    <row r="58" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="15" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="s">
+      <c r="B58" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B60" s="0" t="s">
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="15"/>
+      <c r="B59" s="0"/>
+    </row>
+    <row r="60" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="13" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="B61" s="7" t="s">
         <v>247</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="15" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="15" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="15" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="B65" s="0" t="s">
         <v>255</v>
       </c>
+      <c r="B65" s="7" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="15"/>
-      <c r="B66" s="7"/>
+      <c r="A66" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="15"/>
-      <c r="B67" s="0"/>
-    </row>
-    <row r="68" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B67" s="7"/>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="15"/>
+      <c r="B68" s="0"/>
+    </row>
+    <row r="69" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A42:B42"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update design package for rev-c
Signed-off-by: Grant Likely <grant.likely@linaro.org>
</commit_message>
<xml_diff>
--- a/Sensors-bom-test.xlsx
+++ b/Sensors-bom-test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="263">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -145,7 +145,7 @@
     <t>D2 D9 D10</t>
   </si>
   <si>
-    <t>A</t>
+    <t>PWR A B</t>
   </si>
   <si>
     <t>19-217-G7C-AN1P2-3T</t>
@@ -314,6 +314,21 @@
   </si>
   <si>
     <t>RC0603FR-0710KL</t>
+  </si>
+  <si>
+    <t>S1 S2</t>
+  </si>
+  <si>
+    <t>PWR RST</t>
+  </si>
+  <si>
+    <t>kicad-gcl:SW_PUSH_B3U_1000P</t>
+  </si>
+  <si>
+    <t>Omron</t>
+  </si>
+  <si>
+    <t>B3U-1000P-2P-SMD</t>
   </si>
   <si>
     <t>U1</t>
@@ -961,15 +976,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>390240</xdr:colOff>
+      <xdr:colOff>444240</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>176400</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4208040</xdr:colOff>
+      <xdr:colOff>4261320</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>70560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -982,8 +997,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="390240" y="16395480"/>
-          <a:ext cx="5081760" cy="5246640"/>
+          <a:off x="444240" y="16377480"/>
+          <a:ext cx="5081040" cy="5245920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1003,10 +1018,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1258,7 +1273,7 @@
         <v>304090042</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>41</v>
       </c>
@@ -1614,64 +1629,64 @@
         <v>301010299</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
         <v>99</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="8" t="s">
         <v>101</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F29" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="G29" s="0" t="n">
-        <v>310030097</v>
+      <c r="F29" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29" s="7" t="n">
+        <v>311020047</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="E30" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F30" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="F30" s="0" t="s">
-        <v>106</v>
-      </c>
       <c r="G30" s="0" t="n">
-        <v>310030016</v>
+        <v>310030097</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>110</v>
@@ -1680,7 +1695,7 @@
         <v>111</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>310070030</v>
+        <v>310030016</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1700,116 +1715,124 @@
         <v>115</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>310050024</v>
+        <v>310070030</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>118</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>310050026</v>
+        <v>310050024</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="B34" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C34" s="0" t="s">
+      <c r="E34" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>115</v>
-      </c>
       <c r="F34" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>310050026</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="G35" s="0" t="n">
+    </row>
+    <row r="36" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="G36" s="0" t="n">
         <v>306010054</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7"/>
-      <c r="B36" s="0"/>
-      <c r="D36" s="0"/>
-      <c r="F36" s="0"/>
-      <c r="G36" s="9"/>
-    </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="0"/>
       <c r="D37" s="0"/>
       <c r="F37" s="0"/>
       <c r="G37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B38" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="4"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="F38" s="0"/>
+      <c r="G38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
-        <v>128</v>
+      <c r="A39" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4"/>
@@ -1817,61 +1840,76 @@
       <c r="G39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0"/>
-      <c r="F40" s="0"/>
+      <c r="A40" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>133</v>
-      </c>
+      <c r="A41" s="0"/>
+      <c r="F41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>134</v>
+      <c r="A42" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>137</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1905,7 +1943,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B1" s="0"/>
     </row>
@@ -1920,23 +1958,23 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B6" s="11" t="n">
         <v>2</v>
@@ -1944,63 +1982,63 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B14" s="11"/>
     </row>
@@ -2035,7 +2073,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B1" s="0"/>
     </row>
@@ -2051,7 +2089,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B4" s="0"/>
     </row>
@@ -2061,13 +2099,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B7" s="14"/>
     </row>
@@ -2077,16 +2115,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2095,37 +2133,37 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="B14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B17" s="0"/>
     </row>
@@ -2135,174 +2173,174 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="15" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="15" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="15" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="15" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="15" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="15" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="15" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="15" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="15" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="15" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="15" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="15" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="15" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="15" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="15" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,7 +2349,7 @@
     </row>
     <row r="42" s="12" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B42" s="16"/>
     </row>
@@ -2321,24 +2359,24 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="15" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="15" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="15" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2347,88 +2385,88 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="13" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="15" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="15" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="15" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="15" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="15" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="15" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="15" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="15" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="15" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="15" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2437,58 +2475,58 @@
     </row>
     <row r="60" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="13" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="15" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="15" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="15" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="15" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2501,10 +2539,10 @@
     </row>
     <row r="69" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="15" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove pca9306 from BOM
The 9306 level shifter isn't used in the design, so it shouldn't be in the BOM

Signed-off-by: Grant Likely <grant.likely@linaro.org>
</commit_message>
<xml_diff>
--- a/Sensors-bom-test.xlsx
+++ b/Sensors-bom-test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="976" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,11 +13,16 @@
     <sheet name="Test" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="259">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -389,18 +394,6 @@
   </si>
   <si>
     <t>TXS0108EPWR</t>
-  </si>
-  <si>
-    <t>U6 U7</t>
-  </si>
-  <si>
-    <t>PCA9306</t>
-  </si>
-  <si>
-    <t>Sensors:VSSOP-8_2.4x2.1mm_Pitch0.5mm</t>
-  </si>
-  <si>
-    <t>PCA9306DCU</t>
   </si>
   <si>
     <t>X1</t>
@@ -976,15 +969,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>444240</xdr:colOff>
+      <xdr:colOff>471240</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>158400</xdr:rowOff>
+      <xdr:rowOff>149400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4261320</xdr:colOff>
+      <xdr:colOff>4287960</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -997,8 +990,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="444240" y="16377480"/>
-          <a:ext cx="5081040" cy="5245920"/>
+          <a:off x="471240" y="16368480"/>
+          <a:ext cx="5112000" cy="5245560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1018,23 +1011,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.3296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.24074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="34.4925925925926"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.7"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.3"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.83333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.29259259259259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="35.3740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,7 +1765,7 @@
         <v>124</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>125</v>
@@ -1781,58 +1774,53 @@
         <v>126</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="G36" s="0" t="n">
+      <c r="G35" s="0" t="n">
         <v>306010054</v>
       </c>
     </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7"/>
+      <c r="B36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="F36" s="0"/>
+      <c r="G36" s="9"/>
+    </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="0"/>
       <c r="D37" s="0"/>
       <c r="F37" s="0"/>
       <c r="G37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10"/>
-      <c r="B38" s="0"/>
-      <c r="D38" s="0"/>
-      <c r="F38" s="0"/>
-      <c r="G38" s="9"/>
+      <c r="A38" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
-        <v>133</v>
+      <c r="A39" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4"/>
@@ -1840,76 +1828,61 @@
       <c r="G39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="0"/>
+      <c r="F40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E41" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="B40" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C40" s="4" t="s">
+      <c r="F41" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="4"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0"/>
-      <c r="F41" s="0"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="s">
+      <c r="F42" s="11" t="s">
         <v>136</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1936,14 +1909,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.837037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.83333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B1" s="0"/>
     </row>
@@ -1958,23 +1931,23 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B6" s="11" t="n">
         <v>2</v>
@@ -1982,63 +1955,63 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B14" s="11"/>
     </row>
@@ -2066,14 +2039,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="13.0074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="52.1444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.83333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="13.3259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="53.4074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B1" s="0"/>
     </row>
@@ -2089,7 +2062,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B4" s="0"/>
     </row>
@@ -2099,13 +2072,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B7" s="14"/>
     </row>
@@ -2115,16 +2088,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,37 +2106,37 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B17" s="0"/>
     </row>
@@ -2173,174 +2146,174 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="15" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="15" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="15" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="15" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="15" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="15" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="15" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="15" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="15" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="15" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="15" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="15" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="15" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2349,7 +2322,7 @@
     </row>
     <row r="42" s="12" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B42" s="16"/>
     </row>
@@ -2359,24 +2332,24 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="15" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="15" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,88 +2358,88 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="15" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="15" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="15" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="15" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="15" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="15" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="15" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="15" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="15" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="15" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,58 +2448,58 @@
     </row>
     <row r="60" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="15" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="15" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="15" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="15" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,10 +2512,10 @@
     </row>
     <row r="69" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="15" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove D9, D10, R13, and R14 from the BOM
LEDs D9 and D10 put too much load on the level shifter U4. Remove the
LEDs so that the GPIO lines become usable.

Signed-off-by: Grant Likely <grant.likely@linaro.org>
</commit_message>
<xml_diff>
--- a/Sensors-bom-test.xlsx
+++ b/Sensors-bom-test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="250">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -147,10 +147,10 @@
     <t>19-217-R6C-AL1M2VY-3T</t>
   </si>
   <si>
-    <t>D2 D9 D10</t>
-  </si>
-  <si>
-    <t>PWR A B</t>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>PWR</t>
   </si>
   <si>
     <t>19-217-G7C-AN1P2-3T</t>
@@ -285,7 +285,7 @@
     <t>RC0603JR-07220RL</t>
   </si>
   <si>
-    <t>R2 R3 R4 R13 R14</t>
+    <t>R2 R3 R4</t>
   </si>
   <si>
     <t>1K</t>
@@ -420,40 +420,13 @@
     <t>M2.5 8mm threaded spacer</t>
   </si>
   <si>
-    <t>Changes from Rev B:</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
     <t>Select components as appropriate for cost reductions</t>
   </si>
   <si>
-    <t>C18 changed from 100n to 10u</t>
-  </si>
-  <si>
     <t>Seeed OPL components have been selected where possible</t>
-  </si>
-  <si>
-    <t>C22 added</t>
-  </si>
-  <si>
-    <t>R15 remove</t>
-  </si>
-  <si>
-    <t>R16 R17 R18 R19 changed to 10k</t>
-  </si>
-  <si>
-    <t>Added R23 R24 R25 R26</t>
-  </si>
-  <si>
-    <t>Removed SW1</t>
-  </si>
-  <si>
-    <t>Added S1 S2</t>
-  </si>
-  <si>
-    <t>Q2 Q3 Q4 Q5 change to BSS138</t>
   </si>
   <si>
     <t>PCB Spec</t>
@@ -969,15 +942,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>471240</xdr:colOff>
+      <xdr:colOff>498240</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>149400</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4287960</xdr:colOff>
+      <xdr:colOff>4314600</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>61200</xdr:rowOff>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -990,8 +963,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="471240" y="16368480"/>
-          <a:ext cx="5112000" cy="5245560"/>
+          <a:off x="498240" y="16359480"/>
+          <a:ext cx="5140080" cy="5245200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1011,23 +984,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="1" sqref="F24:F28 F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.29259259259259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="35.3740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.5444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.38888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.2592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,7 +1244,7 @@
         <v>41</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>42</v>
@@ -1535,7 +1508,7 @@
         <v>87</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>88</v>
@@ -1599,7 +1572,7 @@
         <v>301010289</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="31.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
         <v>96</v>
       </c>
@@ -1802,7 +1775,7 @@
         <v>129</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>130</v>
@@ -1832,57 +1805,18 @@
       <c r="F40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="3"/>
+      <c r="E41" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="F41" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="F41" s="11" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0"/>
+      <c r="F42" s="11" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1904,19 +1838,19 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="F24:F28 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.5555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B1" s="0"/>
     </row>
@@ -1931,23 +1865,23 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B6" s="11" t="n">
         <v>2</v>
@@ -1955,63 +1889,63 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B14" s="11"/>
     </row>
@@ -2034,19 +1968,19 @@
   <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="F24:F28 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="13.3259259259259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="53.4074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="13.6222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="54.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B1" s="0"/>
     </row>
@@ -2062,7 +1996,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B4" s="0"/>
     </row>
@@ -2072,13 +2006,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B7" s="14"/>
     </row>
@@ -2088,16 +2022,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,37 +2040,37 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B17" s="0"/>
     </row>
@@ -2146,174 +2080,174 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="15" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="15" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="15" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="15" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="15" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="15" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="15" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="15" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="15" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="15" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="15" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="15" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="15" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="15" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="15" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,7 +2256,7 @@
     </row>
     <row r="42" s="12" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B42" s="16"/>
     </row>
@@ -2332,24 +2266,24 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="15" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="15" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="15" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,88 +2292,88 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="13" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="15" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="15" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="15" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="15" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="15" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="15" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="15" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="15" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="15" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="15" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2448,58 +2382,58 @@
     </row>
     <row r="60" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="13" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="15" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="15" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="15" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="15" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="15" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2512,10 +2446,10 @@
     </row>
     <row r="69" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="15" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>